<commit_message>
Added Db and manual case
</commit_message>
<xml_diff>
--- a/src/main/resources/base/qasayim_template.xlsx
+++ b/src/main/resources/base/qasayim_template.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sum_rules" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="excel_template" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="rules" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="logins" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="94">
   <si>
     <t xml:space="preserve">الجمله</t>
   </si>
@@ -484,6 +485,18 @@
   </si>
   <si>
     <t xml:space="preserve">حاله يدويه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2KzZhdin2YQK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2LPZhdix2YcK</t>
   </si>
 </sst>
 </file>
@@ -714,11 +727,11 @@
   </sheetPr>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="BW3" activeCellId="0" sqref="BW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.5"/>
@@ -1075,11 +1088,11 @@
   </sheetPr>
   <dimension ref="A1:BB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="W3" activeCellId="0" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.5"/>
@@ -1612,11 +1625,11 @@
   </sheetPr>
   <dimension ref="A1:BB36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="72.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.5"/>
@@ -7318,4 +7331,44 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>